<commit_message>
added name thingy for files
</commit_message>
<xml_diff>
--- a/result_file.xlsx
+++ b/result_file.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,6 +509,21 @@
           <t>(2전공 )바이오생활공학 전선</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>(부)문화미디어 전기</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>(부)문화미디어 전필</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>(부)문화미디어 전선</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -558,6 +573,15 @@
       <c r="O2" t="n">
         <v>15</v>
       </c>
+      <c r="P2" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -609,6 +633,15 @@
       <c r="O3" t="n">
         <v>0</v>
       </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -656,6 +689,15 @@
         <v>12</v>
       </c>
       <c r="O4" t="n">
+        <v>15</v>
+      </c>
+      <c r="P4" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>